<commit_message>
Base file with dynamic pages after login page
</commit_message>
<xml_diff>
--- a/media/Employees/Employee_Database.xlsx
+++ b/media/Employees/Employee_Database.xlsx
@@ -2750,12 +2750,12 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>MAGMA</t>
+          <t>FULLERTON</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>AUTO</t>
+          <t>RECOVERY</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">

</xml_diff>

<commit_message>
MAGMA-AUTO MIS AND BILLING OK-1
</commit_message>
<xml_diff>
--- a/media/Employees/Employee_Database.xlsx
+++ b/media/Employees/Employee_Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohaksehgal/Website_Deployment/media/Employees/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA902B7D-08FC-B447-9C97-D45808053F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12270AC0-B09B-A649-BBF1-7563E19EB86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1503,7 +1503,7 @@
   <dimension ref="A1:R159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Some Change in SLICE-CC-1
</commit_message>
<xml_diff>
--- a/media/Employees/Employee_Database.xlsx
+++ b/media/Employees/Employee_Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohaksehgal/Documents/Website/media/Employees/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01F5FB4-15BD-8D44-929E-5D080F6F6751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DAAC80-2027-BE45-98E0-A2FFC4C780B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1504,7 +1504,7 @@
   <dimension ref="A1:R159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>